<commit_message>
Atualização 30 e 31/05/2020
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3798,6 +3798,118 @@
         <v>9</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>30/05/2020</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>137</v>
+      </c>
+      <c r="D63" t="n">
+        <v>4</v>
+      </c>
+      <c r="E63" t="n">
+        <v>32</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>90,19804066</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>0,02919708029</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>101</v>
+      </c>
+      <c r="I63" t="n">
+        <v>285</v>
+      </c>
+      <c r="J63" t="n">
+        <v>422</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>36</v>
+      </c>
+      <c r="M63" t="n">
+        <v>3</v>
+      </c>
+      <c r="N63" t="n">
+        <v>33</v>
+      </c>
+      <c r="O63" t="n">
+        <v>1</v>
+      </c>
+      <c r="P63" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>31/05/2020</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>138</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4</v>
+      </c>
+      <c r="E64" t="n">
+        <v>24</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>90,85642052</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>0,02898550725</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>110</v>
+      </c>
+      <c r="I64" t="n">
+        <v>287</v>
+      </c>
+      <c r="J64" t="n">
+        <v>425</v>
+      </c>
+      <c r="K64" t="n">
+        <v>1</v>
+      </c>
+      <c r="L64" t="n">
+        <v>35</v>
+      </c>
+      <c r="M64" t="n">
+        <v>2</v>
+      </c>
+      <c r="N64" t="n">
+        <v>33</v>
+      </c>
+      <c r="O64" t="n">
+        <v>3</v>
+      </c>
+      <c r="P64" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 10 e 11/06/2020
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R73"/>
+  <dimension ref="A1:R75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4852,6 +4852,130 @@
         <v>11</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>10/06/2020</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>237</v>
+      </c>
+      <c r="D74" t="n">
+        <v>6</v>
+      </c>
+      <c r="E74" t="n">
+        <v>46</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>156,0360265</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0,0253164557</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>184</v>
+      </c>
+      <c r="I74" t="n">
+        <v>410</v>
+      </c>
+      <c r="J74" t="n">
+        <v>647</v>
+      </c>
+      <c r="K74" t="n">
+        <v>10</v>
+      </c>
+      <c r="L74" t="n">
+        <v>50</v>
+      </c>
+      <c r="M74" t="n">
+        <v>5</v>
+      </c>
+      <c r="N74" t="n">
+        <v>45</v>
+      </c>
+      <c r="O74" t="n">
+        <v>23</v>
+      </c>
+      <c r="P74" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>9</v>
+      </c>
+      <c r="R74" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>11/06/2020</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>246</v>
+      </c>
+      <c r="D75" t="n">
+        <v>7</v>
+      </c>
+      <c r="E75" t="n">
+        <v>42</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>161,9614453</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>0,02845528455</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>196</v>
+      </c>
+      <c r="I75" t="n">
+        <v>434</v>
+      </c>
+      <c r="J75" t="n">
+        <v>680</v>
+      </c>
+      <c r="K75" t="n">
+        <v>9</v>
+      </c>
+      <c r="L75" t="n">
+        <v>48</v>
+      </c>
+      <c r="M75" t="n">
+        <v>5</v>
+      </c>
+      <c r="N75" t="n">
+        <v>43</v>
+      </c>
+      <c r="O75" t="n">
+        <v>33</v>
+      </c>
+      <c r="P75" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>9</v>
+      </c>
+      <c r="R75" t="n">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 30/06/2020 - 01/07/2020
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6092,6 +6092,130 @@
         <v>14</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>30/06/2020</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>701</v>
+      </c>
+      <c r="D94" t="n">
+        <v>19</v>
+      </c>
+      <c r="E94" t="n">
+        <v>112</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>461,524281</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>0,02710413695</t>
+        </is>
+      </c>
+      <c r="H94" t="n">
+        <v>567</v>
+      </c>
+      <c r="I94" t="n">
+        <v>925</v>
+      </c>
+      <c r="J94" t="n">
+        <v>1626</v>
+      </c>
+      <c r="K94" t="n">
+        <v>35</v>
+      </c>
+      <c r="L94" t="n">
+        <v>53</v>
+      </c>
+      <c r="M94" t="n">
+        <v>5</v>
+      </c>
+      <c r="N94" t="n">
+        <v>48</v>
+      </c>
+      <c r="O94" t="n">
+        <v>94</v>
+      </c>
+      <c r="P94" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>14</v>
+      </c>
+      <c r="R94" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>733</v>
+      </c>
+      <c r="D95" t="n">
+        <v>21</v>
+      </c>
+      <c r="E95" t="n">
+        <v>126</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>482,5924365</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>0,02864938608</t>
+        </is>
+      </c>
+      <c r="H95" t="n">
+        <v>583</v>
+      </c>
+      <c r="I95" t="n">
+        <v>989</v>
+      </c>
+      <c r="J95" t="n">
+        <v>1722</v>
+      </c>
+      <c r="K95" t="n">
+        <v>32</v>
+      </c>
+      <c r="L95" t="n">
+        <v>46</v>
+      </c>
+      <c r="M95" t="n">
+        <v>4</v>
+      </c>
+      <c r="N95" t="n">
+        <v>42</v>
+      </c>
+      <c r="O95" t="n">
+        <v>96</v>
+      </c>
+      <c r="P95" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>14</v>
+      </c>
+      <c r="R95" t="n">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 06 e 07/07/2020
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6464,6 +6464,130 @@
         <v>15</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>06/07/2020</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>919</v>
+      </c>
+      <c r="D100" t="n">
+        <v>24</v>
+      </c>
+      <c r="E100" t="n">
+        <v>124</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>605,0510903</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>0,02611534276</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>767</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1197</v>
+      </c>
+      <c r="J100" t="n">
+        <v>2116</v>
+      </c>
+      <c r="K100" t="n">
+        <v>23</v>
+      </c>
+      <c r="L100" t="n">
+        <v>51</v>
+      </c>
+      <c r="M100" t="n">
+        <v>4</v>
+      </c>
+      <c r="N100" t="n">
+        <v>47</v>
+      </c>
+      <c r="O100" t="n">
+        <v>66</v>
+      </c>
+      <c r="P100" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>18</v>
+      </c>
+      <c r="R100" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>07/07/2020</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>947</v>
+      </c>
+      <c r="D101" t="n">
+        <v>24</v>
+      </c>
+      <c r="E101" t="n">
+        <v>119</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>623,4857263</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>0,02534318902</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>800</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1219</v>
+      </c>
+      <c r="J101" t="n">
+        <v>2166</v>
+      </c>
+      <c r="K101" t="n">
+        <v>28</v>
+      </c>
+      <c r="L101" t="n">
+        <v>54</v>
+      </c>
+      <c r="M101" t="n">
+        <v>4</v>
+      </c>
+      <c r="N101" t="n">
+        <v>50</v>
+      </c>
+      <c r="O101" t="n">
+        <v>50</v>
+      </c>
+      <c r="P101" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>17</v>
+      </c>
+      <c r="R101" t="n">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
To de volta caraiooo
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q250"/>
+  <dimension ref="A1:Q263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14078,6 +14078,721 @@
         <v>36</v>
       </c>
     </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>04/12/2020</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>250</v>
+      </c>
+      <c r="C251" t="n">
+        <v>3968</v>
+      </c>
+      <c r="D251" t="n">
+        <v>100</v>
+      </c>
+      <c r="E251" t="n">
+        <v>81</v>
+      </c>
+      <c r="F251" t="n">
+        <v>0.0252016129032258</v>
+      </c>
+      <c r="G251" t="n">
+        <v>3770</v>
+      </c>
+      <c r="H251" t="n">
+        <v>12548</v>
+      </c>
+      <c r="I251" t="n">
+        <v>16516</v>
+      </c>
+      <c r="J251" t="n">
+        <v>44</v>
+      </c>
+      <c r="K251" t="n">
+        <v>313</v>
+      </c>
+      <c r="L251" t="n">
+        <v>1</v>
+      </c>
+      <c r="M251" t="n">
+        <v>312</v>
+      </c>
+      <c r="N251" t="n">
+        <v>164</v>
+      </c>
+      <c r="O251" t="n">
+        <v>25</v>
+      </c>
+      <c r="P251" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q251" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>05/12/2020</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>251</v>
+      </c>
+      <c r="C252" t="n">
+        <v>4007</v>
+      </c>
+      <c r="D252" t="n">
+        <v>100</v>
+      </c>
+      <c r="E252" t="n">
+        <v>58</v>
+      </c>
+      <c r="F252" t="n">
+        <v>0.02495632642874969</v>
+      </c>
+      <c r="G252" t="n">
+        <v>3832</v>
+      </c>
+      <c r="H252" t="n">
+        <v>12608</v>
+      </c>
+      <c r="I252" t="n">
+        <v>16615</v>
+      </c>
+      <c r="J252" t="n">
+        <v>39</v>
+      </c>
+      <c r="K252" t="n">
+        <v>248</v>
+      </c>
+      <c r="L252" t="n">
+        <v>2</v>
+      </c>
+      <c r="M252" t="n">
+        <v>246</v>
+      </c>
+      <c r="N252" t="n">
+        <v>99</v>
+      </c>
+      <c r="O252" t="n">
+        <v>19</v>
+      </c>
+      <c r="P252" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q252" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>06/12/2020</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>252</v>
+      </c>
+      <c r="C253" t="n">
+        <v>4029</v>
+      </c>
+      <c r="D253" t="n">
+        <v>100</v>
+      </c>
+      <c r="E253" t="n">
+        <v>48</v>
+      </c>
+      <c r="F253" t="n">
+        <v>0.02482005460412013</v>
+      </c>
+      <c r="G253" t="n">
+        <v>3864</v>
+      </c>
+      <c r="H253" t="n">
+        <v>12680</v>
+      </c>
+      <c r="I253" t="n">
+        <v>16709</v>
+      </c>
+      <c r="J253" t="n">
+        <v>22</v>
+      </c>
+      <c r="K253" t="n">
+        <v>226</v>
+      </c>
+      <c r="L253" t="n">
+        <v>4</v>
+      </c>
+      <c r="M253" t="n">
+        <v>222</v>
+      </c>
+      <c r="N253" t="n">
+        <v>94</v>
+      </c>
+      <c r="O253" t="n">
+        <v>15</v>
+      </c>
+      <c r="P253" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q253" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>07/12/2020</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>253</v>
+      </c>
+      <c r="C254" t="n">
+        <v>4049</v>
+      </c>
+      <c r="D254" t="n">
+        <v>100</v>
+      </c>
+      <c r="E254" t="n">
+        <v>35</v>
+      </c>
+      <c r="F254" t="n">
+        <v>0.02469745616201531</v>
+      </c>
+      <c r="G254" t="n">
+        <v>3897</v>
+      </c>
+      <c r="H254" t="n">
+        <v>12680</v>
+      </c>
+      <c r="I254" t="n">
+        <v>16729</v>
+      </c>
+      <c r="J254" t="n">
+        <v>20</v>
+      </c>
+      <c r="K254" t="n">
+        <v>234</v>
+      </c>
+      <c r="L254" t="n">
+        <v>5</v>
+      </c>
+      <c r="M254" t="n">
+        <v>229</v>
+      </c>
+      <c r="N254" t="n">
+        <v>20</v>
+      </c>
+      <c r="O254" t="n">
+        <v>15</v>
+      </c>
+      <c r="P254" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q254" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>08/12/2020</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>254</v>
+      </c>
+      <c r="C255" t="n">
+        <v>4076</v>
+      </c>
+      <c r="D255" t="n">
+        <v>100</v>
+      </c>
+      <c r="E255" t="n">
+        <v>41</v>
+      </c>
+      <c r="F255" t="n">
+        <v>0.02453385672227674</v>
+      </c>
+      <c r="G255" t="n">
+        <v>3918</v>
+      </c>
+      <c r="H255" t="n">
+        <v>12704</v>
+      </c>
+      <c r="I255" t="n">
+        <v>16780</v>
+      </c>
+      <c r="J255" t="n">
+        <v>27</v>
+      </c>
+      <c r="K255" t="n">
+        <v>183</v>
+      </c>
+      <c r="L255" t="n">
+        <v>6</v>
+      </c>
+      <c r="M255" t="n">
+        <v>177</v>
+      </c>
+      <c r="N255" t="n">
+        <v>51</v>
+      </c>
+      <c r="O255" t="n">
+        <v>14</v>
+      </c>
+      <c r="P255" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q255" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>09/12/2020</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>255</v>
+      </c>
+      <c r="C256" t="n">
+        <v>4097</v>
+      </c>
+      <c r="D256" t="n">
+        <v>100</v>
+      </c>
+      <c r="E256" t="n">
+        <v>46</v>
+      </c>
+      <c r="F256" t="n">
+        <v>0.0244081034903588</v>
+      </c>
+      <c r="G256" t="n">
+        <v>3934</v>
+      </c>
+      <c r="H256" t="n">
+        <v>12801</v>
+      </c>
+      <c r="I256" t="n">
+        <v>16898</v>
+      </c>
+      <c r="J256" t="n">
+        <v>21</v>
+      </c>
+      <c r="K256" t="n">
+        <v>276</v>
+      </c>
+      <c r="L256" t="n">
+        <v>6</v>
+      </c>
+      <c r="M256" t="n">
+        <v>270</v>
+      </c>
+      <c r="N256" t="n">
+        <v>118</v>
+      </c>
+      <c r="O256" t="n">
+        <v>18</v>
+      </c>
+      <c r="P256" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q256" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>10/12/2020</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>256</v>
+      </c>
+      <c r="C257" t="n">
+        <v>4141</v>
+      </c>
+      <c r="D257" t="n">
+        <v>100</v>
+      </c>
+      <c r="E257" t="n">
+        <v>59</v>
+      </c>
+      <c r="F257" t="n">
+        <v>0.02414875633904854</v>
+      </c>
+      <c r="G257" t="n">
+        <v>3965</v>
+      </c>
+      <c r="H257" t="n">
+        <v>12925</v>
+      </c>
+      <c r="I257" t="n">
+        <v>17066</v>
+      </c>
+      <c r="J257" t="n">
+        <v>44</v>
+      </c>
+      <c r="K257" t="n">
+        <v>221</v>
+      </c>
+      <c r="L257" t="n">
+        <v>7</v>
+      </c>
+      <c r="M257" t="n">
+        <v>214</v>
+      </c>
+      <c r="N257" t="n">
+        <v>168</v>
+      </c>
+      <c r="O257" t="n">
+        <v>20</v>
+      </c>
+      <c r="P257" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q257" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>11/12/2020</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>257</v>
+      </c>
+      <c r="C258" t="n">
+        <v>4180</v>
+      </c>
+      <c r="D258" t="n">
+        <v>101</v>
+      </c>
+      <c r="E258" t="n">
+        <v>66</v>
+      </c>
+      <c r="F258" t="n">
+        <v>0.02416267942583732</v>
+      </c>
+      <c r="G258" t="n">
+        <v>3996</v>
+      </c>
+      <c r="H258" t="n">
+        <v>12963</v>
+      </c>
+      <c r="I258" t="n">
+        <v>17143</v>
+      </c>
+      <c r="J258" t="n">
+        <v>39</v>
+      </c>
+      <c r="K258" t="n">
+        <v>314</v>
+      </c>
+      <c r="L258" t="n">
+        <v>2</v>
+      </c>
+      <c r="M258" t="n">
+        <v>312</v>
+      </c>
+      <c r="N258" t="n">
+        <v>77</v>
+      </c>
+      <c r="O258" t="n">
+        <v>18</v>
+      </c>
+      <c r="P258" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q258" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>12/12/2020</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>258</v>
+      </c>
+      <c r="C259" t="n">
+        <v>4180</v>
+      </c>
+      <c r="D259" t="n">
+        <v>101</v>
+      </c>
+      <c r="E259" t="n">
+        <v>66</v>
+      </c>
+      <c r="F259" t="n">
+        <v>0.02416267942583732</v>
+      </c>
+      <c r="G259" t="n">
+        <v>3996</v>
+      </c>
+      <c r="H259" t="n">
+        <v>12963</v>
+      </c>
+      <c r="I259" t="n">
+        <v>17143</v>
+      </c>
+      <c r="J259" t="n">
+        <v>0</v>
+      </c>
+      <c r="K259" t="n">
+        <v>314</v>
+      </c>
+      <c r="L259" t="n">
+        <v>2</v>
+      </c>
+      <c r="M259" t="n">
+        <v>312</v>
+      </c>
+      <c r="N259" t="n">
+        <v>0</v>
+      </c>
+      <c r="O259" t="n">
+        <v>18</v>
+      </c>
+      <c r="P259" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q259" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>13/12/2020</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>259</v>
+      </c>
+      <c r="C260" t="n">
+        <v>4185</v>
+      </c>
+      <c r="D260" t="n">
+        <v>101</v>
+      </c>
+      <c r="E260" t="n">
+        <v>33</v>
+      </c>
+      <c r="F260" t="n">
+        <v>0.02413381123058542</v>
+      </c>
+      <c r="G260" t="n">
+        <v>4034</v>
+      </c>
+      <c r="H260" t="n">
+        <v>12974</v>
+      </c>
+      <c r="I260" t="n">
+        <v>17159</v>
+      </c>
+      <c r="J260" t="n">
+        <v>5</v>
+      </c>
+      <c r="K260" t="n">
+        <v>316</v>
+      </c>
+      <c r="L260" t="n">
+        <v>3</v>
+      </c>
+      <c r="M260" t="n">
+        <v>313</v>
+      </c>
+      <c r="N260" t="n">
+        <v>16</v>
+      </c>
+      <c r="O260" t="n">
+        <v>19</v>
+      </c>
+      <c r="P260" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q260" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>14/12/2020</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>260</v>
+      </c>
+      <c r="C261" t="n">
+        <v>4185</v>
+      </c>
+      <c r="D261" t="n">
+        <v>101</v>
+      </c>
+      <c r="E261" t="n">
+        <v>33</v>
+      </c>
+      <c r="F261" t="n">
+        <v>0.02413381123058542</v>
+      </c>
+      <c r="G261" t="n">
+        <v>4034</v>
+      </c>
+      <c r="H261" t="n">
+        <v>12974</v>
+      </c>
+      <c r="I261" t="n">
+        <v>17159</v>
+      </c>
+      <c r="J261" t="n">
+        <v>0</v>
+      </c>
+      <c r="K261" t="n">
+        <v>316</v>
+      </c>
+      <c r="L261" t="n">
+        <v>3</v>
+      </c>
+      <c r="M261" t="n">
+        <v>313</v>
+      </c>
+      <c r="N261" t="n">
+        <v>0</v>
+      </c>
+      <c r="O261" t="n">
+        <v>19</v>
+      </c>
+      <c r="P261" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q261" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>15/12/2020</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>261</v>
+      </c>
+      <c r="C262" t="n">
+        <v>4228</v>
+      </c>
+      <c r="D262" t="n">
+        <v>102</v>
+      </c>
+      <c r="E262" t="n">
+        <v>36</v>
+      </c>
+      <c r="F262" t="n">
+        <v>0.02412488174077578</v>
+      </c>
+      <c r="G262" t="n">
+        <v>4073</v>
+      </c>
+      <c r="H262" t="n">
+        <v>13076</v>
+      </c>
+      <c r="I262" t="n">
+        <v>17304</v>
+      </c>
+      <c r="J262" t="n">
+        <v>43</v>
+      </c>
+      <c r="K262" t="n">
+        <v>446</v>
+      </c>
+      <c r="L262" t="n">
+        <v>1</v>
+      </c>
+      <c r="M262" t="n">
+        <v>445</v>
+      </c>
+      <c r="N262" t="n">
+        <v>145</v>
+      </c>
+      <c r="O262" t="n">
+        <v>21</v>
+      </c>
+      <c r="P262" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q262" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>16/12/2020</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>262</v>
+      </c>
+      <c r="C263" t="n">
+        <v>4262</v>
+      </c>
+      <c r="D263" t="n">
+        <v>102</v>
+      </c>
+      <c r="E263" t="n">
+        <v>38</v>
+      </c>
+      <c r="F263" t="n">
+        <v>0.02393242609103707</v>
+      </c>
+      <c r="G263" t="n">
+        <v>4105</v>
+      </c>
+      <c r="H263" t="n">
+        <v>13173</v>
+      </c>
+      <c r="I263" t="n">
+        <v>17435</v>
+      </c>
+      <c r="J263" t="n">
+        <v>34</v>
+      </c>
+      <c r="K263" t="n">
+        <v>435</v>
+      </c>
+      <c r="L263" t="n">
+        <v>2</v>
+      </c>
+      <c r="M263" t="n">
+        <v>434</v>
+      </c>
+      <c r="N263" t="n">
+        <v>131</v>
+      </c>
+      <c r="O263" t="n">
+        <v>16</v>
+      </c>
+      <c r="P263" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q263" t="n">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de volta a ativa
</commit_message>
<xml_diff>
--- a/Dados/dadosCasosCOVIDMogiGuacu.xlsx
+++ b/Dados/dadosCasosCOVIDMogiGuacu.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R285"/>
+  <dimension ref="A1:R288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16860,6 +16860,180 @@
         <v>41</v>
       </c>
     </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>08/01/2021</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>285</v>
+      </c>
+      <c r="C286" t="n">
+        <v>5210</v>
+      </c>
+      <c r="D286" t="n">
+        <v>120</v>
+      </c>
+      <c r="E286" t="n">
+        <v>161</v>
+      </c>
+      <c r="F286" t="n">
+        <v>0.02303262955854127</v>
+      </c>
+      <c r="G286" t="n">
+        <v>4911</v>
+      </c>
+      <c r="H286" t="n">
+        <v>14698</v>
+      </c>
+      <c r="I286" t="n">
+        <v>19908</v>
+      </c>
+      <c r="J286" t="n">
+        <v>85</v>
+      </c>
+      <c r="K286" t="n">
+        <v>490</v>
+      </c>
+      <c r="L286" t="n">
+        <v>1</v>
+      </c>
+      <c r="M286" t="n">
+        <v>489</v>
+      </c>
+      <c r="N286" t="n">
+        <v>193</v>
+      </c>
+      <c r="O286" t="n">
+        <v>25</v>
+      </c>
+      <c r="P286" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q286" t="n">
+        <v>4</v>
+      </c>
+      <c r="R286" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>09/01/2021</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>286</v>
+      </c>
+      <c r="C287" t="n">
+        <v>5252</v>
+      </c>
+      <c r="D287" t="n">
+        <v>120</v>
+      </c>
+      <c r="E287" t="n">
+        <v>133</v>
+      </c>
+      <c r="F287" t="n">
+        <v>0.02284843869002285</v>
+      </c>
+      <c r="G287" t="n">
+        <v>4981</v>
+      </c>
+      <c r="H287" t="n">
+        <v>14760</v>
+      </c>
+      <c r="I287" t="n">
+        <v>20012</v>
+      </c>
+      <c r="J287" t="n">
+        <v>42</v>
+      </c>
+      <c r="K287" t="n">
+        <v>468</v>
+      </c>
+      <c r="L287" t="n">
+        <v>2</v>
+      </c>
+      <c r="M287" t="n">
+        <v>466</v>
+      </c>
+      <c r="N287" t="n">
+        <v>104</v>
+      </c>
+      <c r="O287" t="n">
+        <v>28</v>
+      </c>
+      <c r="P287" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q287" t="n">
+        <v>0</v>
+      </c>
+      <c r="R287" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>10/01/2021</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>287</v>
+      </c>
+      <c r="C288" t="n">
+        <v>5265</v>
+      </c>
+      <c r="D288" t="n">
+        <v>120</v>
+      </c>
+      <c r="E288" t="n">
+        <v>108</v>
+      </c>
+      <c r="F288" t="n">
+        <v>0.02279202279202279</v>
+      </c>
+      <c r="G288" t="n">
+        <v>5019</v>
+      </c>
+      <c r="H288" t="n">
+        <v>14760</v>
+      </c>
+      <c r="I288" t="n">
+        <v>20025</v>
+      </c>
+      <c r="J288" t="n">
+        <v>13</v>
+      </c>
+      <c r="K288" t="n">
+        <v>469</v>
+      </c>
+      <c r="L288" t="n">
+        <v>3</v>
+      </c>
+      <c r="M288" t="n">
+        <v>466</v>
+      </c>
+      <c r="N288" t="n">
+        <v>13</v>
+      </c>
+      <c r="O288" t="n">
+        <v>26</v>
+      </c>
+      <c r="P288" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q288" t="n">
+        <v>0</v>
+      </c>
+      <c r="R288" t="n">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>